<commit_message>
final project ver 1.0.1.2
</commit_message>
<xml_diff>
--- a/ExcelFiles/books.xlsx
+++ b/ExcelFiles/books.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,34 +441,68 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Title</t>
+          <t>applebees</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Genre</t>
+          <t>nonfiction</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Volumes</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>scott</t>
+          <t>dragon ball</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>son2</t>
+          <t>manga</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2222</t>
+          <t>1,2,3,4,5,6,7</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>naruto</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>manga</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>man</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
final project ver 1.0.1.2 added requirements.txt
</commit_message>
<xml_diff>
--- a/ExcelFiles/books.xlsx
+++ b/ExcelFiles/books.xlsx
@@ -446,36 +446,36 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>fiction</t>
+          <t>nonfiction</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>d</t>
+          <t>dragon ball</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>man</t>
+          <t>manga</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1,2,3,4,5,6,7</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>dragon ball</t>
+          <t>naruto</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -485,14 +485,14 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1,2,3,4,5,6,7</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>naruto</t>
+          <t>d</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">

</xml_diff>

<commit_message>
final project ver 1.0.1.4 added requirements.txt changed some functionality added  save and delete buttons and wrpaped the other buttons around
fixed an issue where if you had multiple volumes it does not populate the text boxes.
</commit_message>
<xml_diff>
--- a/ExcelFiles/books.xlsx
+++ b/ExcelFiles/books.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,85 +441,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>dragon ball</t>
+          <t>scott</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>manga</t>
+          <t>son</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1,2,3,4,5,6,7</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>naruto</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>manga</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>d</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>manga</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>dragonbody</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>manga</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>applebees</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>nonfiction</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>1,23,4,5</t>
         </is>
       </c>
     </row>

</xml_diff>